<commit_message>
Product Add loop works; still need to add basic price and security handling.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A690F395-0B34-45A8-8970-5AF36BACC6DC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A6A5CA-C4F3-4E53-A3D9-A0310464B9B6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>Setup Price</t>
   </si>
   <si>
-    <t>Dummy Product</t>
-  </si>
-  <si>
     <t>Test product for automation script</t>
   </si>
   <si>
@@ -180,12 +177,6 @@
     <t>carl@classroominabox.com</t>
   </si>
   <si>
-    <t>Test - Dummy Product</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 01</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
   </si>
   <si>
     <t>TEST - Dummy 02</t>
-  </si>
-  <si>
-    <t>Test - Dummy Product #2</t>
   </si>
   <si>
     <t>Dummy Product 2</t>
@@ -269,6 +257,18 @@
       </rPr>
       <t xml:space="preserve"> how to do that yet. Let's see if "quotes" can be included also.</t>
     </r>
+  </si>
+  <si>
+    <t>Test - Dummy Product 2</t>
+  </si>
+  <si>
+    <t>Test - Dummy Product 4</t>
+  </si>
+  <si>
+    <t>Dummy Product 4</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 04</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:AN3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -826,70 +826,67 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="3">
-        <v>42938</v>
       </c>
       <c r="I2" s="3">
         <v>43956</v>
       </c>
       <c r="J2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2">
         <v>15</v>
       </c>
       <c r="P2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="T2">
         <v>100</v>
       </c>
       <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
         <v>44</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>45</v>
       </c>
       <c r="AC2">
         <v>5</v>
       </c>
       <c r="AD2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE2" t="b">
         <v>1</v>
@@ -898,19 +895,19 @@
         <v>5</v>
       </c>
       <c r="AG2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH2">
         <v>4</v>
       </c>
       <c r="AI2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ2">
         <v>12</v>
       </c>
       <c r="AK2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AL2">
         <v>1</v>
@@ -927,58 +924,58 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O3">
         <v>15</v>
       </c>
       <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="T3">
         <v>100</v>
       </c>
       <c r="AA3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" t="s">
         <v>44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>45</v>
       </c>
       <c r="AC3">
         <v>5</v>
       </c>
       <c r="AD3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE3" t="b">
         <v>1</v>
@@ -987,19 +984,19 @@
         <v>5</v>
       </c>
       <c r="AG3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH3">
         <v>4</v>
       </c>
       <c r="AI3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ3">
         <v>1</v>
       </c>
       <c r="AK3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AL3">
         <v>1</v>

</xml_diff>

<commit_message>
Add variable typing in Wait-Link; first attempt at Get-PriceRow, which doesn't work.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CD6E90-B57E-4B18-8396-3B068AB2925F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D70A9D-70F2-4E78-8C46-B029311AB4C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,16 +259,16 @@
     <t>Test - Dummy Product 2</t>
   </si>
   <si>
-    <t>Test - Dummy Product 4</t>
-  </si>
-  <si>
-    <t>Dummy Product 4</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 04</t>
-  </si>
-  <si>
     <t>mis@contoso.com</t>
+  </si>
+  <si>
+    <t>Test - Dummy Product 6</t>
+  </si>
+  <si>
+    <t>Dummy Product 6</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 06</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,13 +826,13 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -871,7 +871,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="T2">
         <v>100</v>
@@ -960,7 +960,7 @@
         <v>48</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="T3">
         <v>100</v>

</xml_diff>

<commit_message>
Still troubleshooting Get-PriceRow. 2
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D70A9D-70F2-4E78-8C46-B029311AB4C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21153EDB-1529-470B-A225-7DB277FB4878}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,13 +262,13 @@
     <t>mis@contoso.com</t>
   </si>
   <si>
-    <t>Test - Dummy Product 6</t>
-  </si>
-  <si>
-    <t>Dummy Product 6</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 06</t>
+    <t>Test - Dummy Product 7</t>
+  </si>
+  <si>
+    <t>Dummy Product 7</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 07</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Get-PriceRow seems to work; testing Set-PriceRow now.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBE8C7E-0AA0-4B9A-B59F-7D7D110A6901}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B48AD-C001-4BFD-98AE-BFE368EC6D5D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,13 +262,13 @@
     <t>mis@contoso.com</t>
   </si>
   <si>
-    <t>Test - Dummy Product 14</t>
-  </si>
-  <si>
-    <t>Dummy Product 14</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 14</t>
+    <t>Test - Dummy Product 15</t>
+  </si>
+  <si>
+    <t>Dummy Product 15</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 15</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Find-Product added; reworking to take Add/Change operation from input data.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B48AD-C001-4BFD-98AE-BFE368EC6D5D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551450A9-004F-4CDD-A612-EDE64CA39D25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Product Name</t>
   </si>
@@ -177,85 +177,9 @@
     <t>n</t>
   </si>
   <si>
-    <t>ft</t>
-  </si>
-  <si>
     <t>TEST - Dummy 02</t>
   </si>
   <si>
-    <t>Dummy Product 2</t>
-  </si>
-  <si>
-    <t>Another test product for automation script</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is a long description. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Supposedly</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> it can contain </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>formatting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, but </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I don't know</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> how to do that yet. Let's see if "quotes" can be included also.</t>
-    </r>
-  </si>
-  <si>
     <t>Test - Dummy Product 2</t>
   </si>
   <si>
@@ -269,13 +193,28 @@
   </si>
   <si>
     <t>TEST - Dummy 15</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Dummy Product # 2</t>
+  </si>
+  <si>
+    <t>In this test, change TA time to 7 days, and add 25 to inventory count.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,21 +234,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,363 +581,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN3"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>43956</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>42</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
       </c>
       <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
         <v>48</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>15</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2">
+      <c r="S2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2">
         <v>100</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>44</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>5</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>45</v>
       </c>
-      <c r="AE2" t="b">
+      <c r="AF2" t="b">
         <v>1</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>5</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>46</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>4</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>12</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>46</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>1</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>2.87</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="S3" s="4"/>
       <c r="T3">
-        <v>100</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC3">
-        <v>5</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF3">
-        <v>5</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3">
-        <v>4</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
-        <v>1.55</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{9D820934-703B-46C6-BF8A-287C2DF21AAB}"/>
-    <hyperlink ref="R3" r:id="rId2" xr:uid="{95FC74E5-90CF-430C-A8BB-2B23FA62D78E}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{9D820934-703B-46C6-BF8A-287C2DF21AAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set-PriceRow fixed; was using FindElementBy instead of FindElementsBy.  Now testing Change operation including Find-Product.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551450A9-004F-4CDD-A612-EDE64CA39D25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDAFDA9-8A8F-46B6-85A4-750AD3264D9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Product Name</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Operation</t>
-  </si>
-  <si>
-    <t>Add</t>
   </si>
   <si>
     <t>Change</t>
@@ -584,7 +581,7 @@
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,28 +840,25 @@
       <c r="AM2">
         <v>1</v>
       </c>
-      <c r="AN2">
-        <v>2.87</v>
-      </c>
       <c r="AO2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K3">
         <v>7</v>

</xml_diff>

<commit_message>
Fix Manage-Product so it checks for potential duplicate product before trying to add.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0033DEA2-17FB-47C2-9C59-2AFFC9DBB286}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649D1CA-6FAE-451D-9306-1C794667BEC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>Product Name</t>
   </si>
@@ -201,10 +201,34 @@
     <t>Test - Pikachu</t>
   </si>
   <si>
-    <t>Test to make sure we can change product name, given correct ID.</t>
-  </si>
-  <si>
     <t>Second name change just for fun.</t>
+  </si>
+  <si>
+    <t>Test - Wooper</t>
+  </si>
+  <si>
+    <t>Test collision avoidance system.  Product add should fail because it's a dupe.</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Don't wake a sleeping snorlax or it will pound you!</t>
+  </si>
+  <si>
+    <t>They make good defenders.</t>
+  </si>
+  <si>
+    <t>test,product,dummy,snorlax</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>feet</t>
   </si>
 </sst>
 </file>
@@ -578,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,19 +787,16 @@
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="3">
-        <v>43956</v>
+        <v>63</v>
       </c>
       <c r="K2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
         <v>47</v>
@@ -801,17 +822,17 @@
       <c r="S2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="T2">
-        <v>100</v>
+      <c r="U2">
+        <v>355</v>
       </c>
       <c r="AB2" t="s">
         <v>42</v>
       </c>
       <c r="AC2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="AD2">
-        <v>5</v>
+        <v>2000</v>
       </c>
       <c r="AE2" t="s">
         <v>44</v>
@@ -820,59 +841,158 @@
         <v>1</v>
       </c>
       <c r="AG2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AH2" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="AI2">
         <v>4</v>
       </c>
       <c r="AJ2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="AK2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AL2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AM2">
         <v>1</v>
       </c>
+      <c r="AN2">
+        <v>999.01</v>
+      </c>
       <c r="AO2">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="3">
+        <v>43956</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3">
+        <v>100</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3">
+        <v>5</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>5</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI3">
+        <v>4</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK3">
+        <v>12</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3">
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4">
         <v>7</v>
       </c>
-      <c r="S3" s="4"/>
-      <c r="T3">
+      <c r="S4" s="4"/>
+      <c r="T4">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{9D820934-703B-46C6-BF8A-287C2DF21AAB}"/>
+    <hyperlink ref="S3" r:id="rId1" xr:uid="{9D820934-703B-46C6-BF8A-287C2DF21AAB}"/>
+    <hyperlink ref="S2" r:id="rId2" xr:uid="{04B5408E-2650-41B2-B6B3-5F034BE2953F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add output when changing details.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649D1CA-6FAE-451D-9306-1C794667BEC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6454B4FA-1B4B-4277-A277-3F9BC58E5F21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Product Name</t>
   </si>
@@ -144,91 +144,49 @@
     <t>Setup Price</t>
   </si>
   <si>
-    <t>C:\Users\Carl\Pictures\cute_moogle_by_negocio_plz-d5dw8o1.png</t>
-  </si>
-  <si>
-    <t>This is a long description. Supposedly it can contain formatting, but I don't know how to do that yet. Let's see if "quotes" can be included also.</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Notes for production folks.</t>
-  </si>
-  <si>
-    <t>test,product,dummy</t>
-  </si>
-  <si>
-    <t>lb</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>Manage Inventory</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>TEST - Dummy 02</t>
   </si>
   <si>
-    <t>mis@contoso.com</t>
-  </si>
-  <si>
-    <t>Dummy Product 15</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 15</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
     <t>Change</t>
   </si>
   <si>
-    <t>Dummy Product # 2</t>
-  </si>
-  <si>
-    <t>Test - Snorlax</t>
-  </si>
-  <si>
-    <t>Test - Pikachu</t>
-  </si>
-  <si>
-    <t>Second name change just for fun.</t>
-  </si>
-  <si>
-    <t>Test - Wooper</t>
-  </si>
-  <si>
-    <t>Test collision avoidance system.  Product add should fail because it's a dupe.</t>
-  </si>
-  <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Don't wake a sleeping snorlax or it will pound you!</t>
-  </si>
-  <si>
-    <t>They make good defenders.</t>
-  </si>
-  <si>
-    <t>test,product,dummy,snorlax</t>
-  </si>
-  <si>
-    <t>foot</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
-    <t>feet</t>
+    <t>TEST - Dummy 01</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 10</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 04</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 05</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 06</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 07</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 08</t>
+  </si>
+  <si>
+    <t>TEST - Dummy 09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST - Dummy 15 </t>
+  </si>
+  <si>
+    <t>mis@contoso.com;supv@contoso.com</t>
   </si>
 </sst>
 </file>
@@ -602,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO4"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +608,7 @@
   <sheetData>
     <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -692,7 +650,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>13</v>
@@ -775,224 +733,188 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="P2">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2">
-        <v>355</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD2">
-        <v>2000</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>3</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI2">
-        <v>4</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK2">
-        <v>8</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
-        <v>999.01</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="3">
-        <v>43956</v>
-      </c>
-      <c r="K3">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" t="s">
-        <v>47</v>
-      </c>
       <c r="P3">
-        <v>15</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3">
-        <v>100</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD3">
-        <v>5</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>5</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI3">
-        <v>4</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK3">
-        <v>12</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM3">
-        <v>1</v>
-      </c>
-      <c r="AO3">
-        <v>0.75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="E4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4">
-        <v>7</v>
-      </c>
-      <c r="S4" s="4"/>
-      <c r="T4">
-        <v>25</v>
+      <c r="O7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10">
+        <v>100</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <v>100</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S3" r:id="rId1" xr:uid="{9D820934-703B-46C6-BF8A-287C2DF21AAB}"/>
-    <hyperlink ref="S2" r:id="rId2" xr:uid="{04B5408E-2650-41B2-B6B3-5F034BE2953F}"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{93468EE8-F3AA-4F41-9394-654161712BA9}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{A125100A-91D9-48A4-83BF-DD423470255A}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{23106B25-0250-4082-923F-819B570BD294}"/>
+    <hyperlink ref="S5" r:id="rId4" xr:uid="{B6180F8A-75D8-4191-8D27-9317A9826261}"/>
+    <hyperlink ref="S6" r:id="rId5" xr:uid="{84B766FB-4056-406D-9EE5-087083E7428F}"/>
+    <hyperlink ref="S7" r:id="rId6" xr:uid="{4C46FDFA-6506-4203-86BF-405D8024C951}"/>
+    <hyperlink ref="S8" r:id="rId7" xr:uid="{6EFD725F-EBCF-4CDC-A84C-6A44BE6729A3}"/>
+    <hyperlink ref="S9" r:id="rId8" xr:uid="{ECF48555-B261-4CBF-9E5D-586F2FE2288A}"/>
+    <hyperlink ref="S10" r:id="rId9" xr:uid="{90E2A75B-8F69-47A1-80C6-ABA64FC836C8}"/>
+    <hyperlink ref="S11" r:id="rId10" xr:uid="{1F97873B-BD51-4BD4-8DE4-D3850D06DE2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle NoSuchElementException from Se when ID not found in current row, as this is perfectly fine with multiple search hits.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6454B4FA-1B4B-4277-A277-3F9BC58E5F21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82510B8F-D954-4258-94BD-7D5665AD926B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Product Name</t>
   </si>
@@ -162,31 +162,13 @@
     <t>TEST - Dummy 01</t>
   </si>
   <si>
-    <t>TEST - Dummy 10</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 04</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 05</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 06</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 07</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 08</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 09</t>
-  </si>
-  <si>
     <t xml:space="preserve">TEST - Dummy 15 </t>
   </si>
   <si>
     <t>mis@contoso.com;supv@contoso.com</t>
+  </si>
+  <si>
+    <t>ID for this product has a trailing space.</t>
   </si>
 </sst>
 </file>
@@ -560,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO11"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +727,7 @@
         <v>100</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -753,7 +735,7 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
         <v>40</v>
@@ -762,7 +744,7 @@
         <v>100</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
@@ -770,7 +752,10 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
       </c>
       <c r="O4" t="s">
         <v>40</v>
@@ -779,142 +764,16 @@
         <v>100</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6">
-        <v>100</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7">
-        <v>100</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8">
-        <v>100</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9">
-        <v>100</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10">
-        <v>100</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11">
-        <v>100</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{93468EE8-F3AA-4F41-9394-654161712BA9}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{A125100A-91D9-48A4-83BF-DD423470255A}"/>
-    <hyperlink ref="S4" r:id="rId3" xr:uid="{23106B25-0250-4082-923F-819B570BD294}"/>
-    <hyperlink ref="S5" r:id="rId4" xr:uid="{B6180F8A-75D8-4191-8D27-9317A9826261}"/>
-    <hyperlink ref="S6" r:id="rId5" xr:uid="{84B766FB-4056-406D-9EE5-087083E7428F}"/>
-    <hyperlink ref="S7" r:id="rId6" xr:uid="{4C46FDFA-6506-4203-86BF-405D8024C951}"/>
-    <hyperlink ref="S8" r:id="rId7" xr:uid="{6EFD725F-EBCF-4CDC-A84C-6A44BE6729A3}"/>
-    <hyperlink ref="S9" r:id="rId8" xr:uid="{ECF48555-B261-4CBF-9E5D-586F2FE2288A}"/>
-    <hyperlink ref="S10" r:id="rId9" xr:uid="{90E2A75B-8F69-47A1-80C6-ABA64FC836C8}"/>
-    <hyperlink ref="S11" r:id="rId10" xr:uid="{1F97873B-BD51-4BD4-8DE4-D3850D06DE2D}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{90E2A75B-8F69-47A1-80C6-ABA64FC836C8}"/>
+    <hyperlink ref="S4" r:id="rId3" xr:uid="{1F97873B-BD51-4BD4-8DE4-D3850D06DE2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data validation for product short name.
</commit_message>
<xml_diff>
--- a/Test_Product_List.xlsx
+++ b/Test_Product_List.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Scripts\Public\Work\DSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCE1722-E5C9-4EB2-B68B-7DEB1395CA8C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D21E12E-C42E-40C3-ABED-7631A4D2B78E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Product Name</t>
   </si>
@@ -147,29 +153,14 @@
     <t>Manage Inventory</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>Operation</t>
-  </si>
-  <si>
-    <t>Change</t>
-  </si>
-  <si>
-    <t>TEST - Dummy 01</t>
-  </si>
-  <si>
-    <t>mis@contoso.com;supv@contoso.com</t>
-  </si>
-  <si>
-    <t>C:\Users\Carl\Pictures\cute_moogle_by_negocio_plz-d5dw8o1.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,14 +172,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,23 +194,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -536,18 +522,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" customWidth="1"/>
@@ -584,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -707,31 +696,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2">
-        <v>100</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{93468EE8-F3AA-4F41-9394-654161712BA9}"/>
-  </hyperlinks>
+  <dataValidations count="1">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Text Length" error="Must be 50 or fewer characters." promptTitle="Test" prompt="Test message" sqref="B1 B2:B1048576" xr:uid="{B4975AE8-8B6D-4631-9891-CDF74C14FADB}">
+      <formula1>50</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>